<commit_message>
Backup QR Scanner data - 19/05/2025, 8:56:05 AM
</commit_message>
<xml_diff>
--- a/backups/Scanner_Pharmacology_2025-05-19T05-08-34.xlsx
+++ b/backups/Scanner_Pharmacology_2025-05-19T05-08-34.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Pharmacology" sheetId="1" r:id="rId1"/>
+    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -430,7 +430,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C2" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D2" t="str">
         <v>08:24:16</v>
@@ -450,7 +450,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C3" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D3" t="str">
         <v>08:24:22</v>
@@ -470,7 +470,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C4" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D4" t="str">
         <v>08:24:34</v>
@@ -490,7 +490,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C5" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D5" t="str">
         <v>08:25:22</v>
@@ -510,7 +510,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C6" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D6" t="str">
         <v>08:25:27</v>
@@ -530,7 +530,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C7" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D7" t="str">
         <v>08:26:20</v>
@@ -550,7 +550,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C8" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D8" t="str">
         <v>08:26:24</v>
@@ -570,7 +570,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C9" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D9" t="str">
         <v>08:26:28</v>
@@ -590,7 +590,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C10" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D10" t="str">
         <v>08:26:30</v>
@@ -610,7 +610,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C11" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D11" t="str">
         <v>08:26:35</v>
@@ -630,7 +630,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C12" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D12" t="str">
         <v>08:26:40</v>
@@ -650,7 +650,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C13" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D13" t="str">
         <v>08:26:45</v>
@@ -670,7 +670,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C14" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D14" t="str">
         <v>08:26:50</v>
@@ -690,7 +690,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C15" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D15" t="str">
         <v>08:26:53</v>
@@ -710,7 +710,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C16" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D16" t="str">
         <v>08:26:57</v>
@@ -730,7 +730,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C17" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D17" t="str">
         <v>08:27:02</v>
@@ -750,7 +750,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C18" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D18" t="str">
         <v>08:27:07</v>
@@ -770,7 +770,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C19" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D19" t="str">
         <v>08:27:12</v>
@@ -790,7 +790,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C20" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D20" t="str">
         <v>08:27:17</v>
@@ -810,7 +810,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C21" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D21" t="str">
         <v>08:27:21</v>
@@ -830,7 +830,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C22" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D22" t="str">
         <v>08:27:24</v>
@@ -850,7 +850,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C23" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D23" t="str">
         <v>08:27:31</v>
@@ -870,7 +870,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C24" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D24" t="str">
         <v>08:27:41</v>
@@ -890,7 +890,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C25" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D25" t="str">
         <v>08:27:46</v>
@@ -910,7 +910,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C26" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D26" t="str">
         <v>08:27:50</v>
@@ -930,7 +930,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C27" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D27" t="str">
         <v>08:27:55</v>
@@ -950,7 +950,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C28" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D28" t="str">
         <v>08:28:00</v>
@@ -970,7 +970,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C29" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D29" t="str">
         <v>08:28:06</v>
@@ -990,7 +990,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C30" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D30" t="str">
         <v>08:28:10</v>
@@ -1010,7 +1010,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C31" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D31" t="str">
         <v>08:28:22</v>
@@ -1030,7 +1030,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C32" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D32" t="str">
         <v>08:28:22</v>
@@ -1050,7 +1050,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C33" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D33" t="str">
         <v>08:28:45</v>
@@ -1070,7 +1070,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C34" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D34" t="str">
         <v>08:29:13</v>
@@ -1090,7 +1090,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C35" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D35" t="str">
         <v>08:29:26</v>
@@ -1110,7 +1110,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C36" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D36" t="str">
         <v>08:29:32</v>
@@ -1130,7 +1130,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C37" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D37" t="str">
         <v>08:29:38</v>
@@ -1150,7 +1150,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C38" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D38" t="str">
         <v>08:29:49</v>
@@ -1170,7 +1170,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C39" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D39" t="str">
         <v>08:29:55</v>
@@ -1190,7 +1190,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C40" t="str">
-        <v>19/05/2025</v>
+        <v>05/19/2025</v>
       </c>
       <c r="D40" t="str">
         <v>08:30:01</v>

</xml_diff>

<commit_message>
Backup QR Scanner data - 19/05/2025, 8:57:29 AM
</commit_message>
<xml_diff>
--- a/backups/Scanner_Pharmacology_2025-05-19T05-08-34.xlsx
+++ b/backups/Scanner_Pharmacology_2025-05-19T05-08-34.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Pharmacology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -430,7 +430,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C2" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D2" t="str">
         <v>08:24:16</v>
@@ -450,7 +450,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C3" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D3" t="str">
         <v>08:24:22</v>
@@ -470,7 +470,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C4" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D4" t="str">
         <v>08:24:34</v>
@@ -490,7 +490,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C5" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D5" t="str">
         <v>08:25:22</v>
@@ -510,7 +510,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C6" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D6" t="str">
         <v>08:25:27</v>
@@ -530,7 +530,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C7" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D7" t="str">
         <v>08:26:20</v>
@@ -550,7 +550,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C8" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D8" t="str">
         <v>08:26:24</v>
@@ -570,7 +570,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C9" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D9" t="str">
         <v>08:26:28</v>
@@ -590,7 +590,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C10" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D10" t="str">
         <v>08:26:30</v>
@@ -610,7 +610,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C11" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D11" t="str">
         <v>08:26:35</v>
@@ -630,7 +630,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C12" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D12" t="str">
         <v>08:26:40</v>
@@ -650,7 +650,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C13" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D13" t="str">
         <v>08:26:45</v>
@@ -670,7 +670,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C14" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D14" t="str">
         <v>08:26:50</v>
@@ -690,7 +690,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C15" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D15" t="str">
         <v>08:26:53</v>
@@ -710,7 +710,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C16" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D16" t="str">
         <v>08:26:57</v>
@@ -730,7 +730,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C17" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D17" t="str">
         <v>08:27:02</v>
@@ -750,7 +750,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C18" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D18" t="str">
         <v>08:27:07</v>
@@ -770,7 +770,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C19" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D19" t="str">
         <v>08:27:12</v>
@@ -790,7 +790,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C20" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D20" t="str">
         <v>08:27:17</v>
@@ -810,7 +810,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C21" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D21" t="str">
         <v>08:27:21</v>
@@ -830,7 +830,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C22" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D22" t="str">
         <v>08:27:24</v>
@@ -850,7 +850,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C23" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D23" t="str">
         <v>08:27:31</v>
@@ -870,7 +870,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C24" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D24" t="str">
         <v>08:27:41</v>
@@ -890,7 +890,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C25" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D25" t="str">
         <v>08:27:46</v>
@@ -910,7 +910,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C26" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D26" t="str">
         <v>08:27:50</v>
@@ -930,7 +930,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C27" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D27" t="str">
         <v>08:27:55</v>
@@ -950,7 +950,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C28" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D28" t="str">
         <v>08:28:00</v>
@@ -970,7 +970,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C29" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D29" t="str">
         <v>08:28:06</v>
@@ -990,7 +990,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C30" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D30" t="str">
         <v>08:28:10</v>
@@ -1010,7 +1010,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C31" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D31" t="str">
         <v>08:28:22</v>
@@ -1030,7 +1030,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C32" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D32" t="str">
         <v>08:28:22</v>
@@ -1050,7 +1050,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C33" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D33" t="str">
         <v>08:28:45</v>
@@ -1070,7 +1070,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C34" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D34" t="str">
         <v>08:29:13</v>
@@ -1090,7 +1090,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C35" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D35" t="str">
         <v>08:29:26</v>
@@ -1110,7 +1110,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C36" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D36" t="str">
         <v>08:29:32</v>
@@ -1130,7 +1130,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C37" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D37" t="str">
         <v>08:29:38</v>
@@ -1150,7 +1150,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C38" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D38" t="str">
         <v>08:29:49</v>
@@ -1170,7 +1170,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C39" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D39" t="str">
         <v>08:29:55</v>
@@ -1190,7 +1190,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C40" t="str">
-        <v>05/19/2025</v>
+        <v>19/05/2025</v>
       </c>
       <c r="D40" t="str">
         <v>08:30:01</v>

</xml_diff>